<commit_message>
fixed revenue report backlog issued
</commit_message>
<xml_diff>
--- a/public/abcd/Crew Stock Report.xlsx
+++ b/public/abcd/Crew Stock Report.xlsx
@@ -26,10 +26,10 @@
     <t>Depot : BALEWADI</t>
   </si>
   <si>
-    <t>From : 01-01-2019</t>
-  </si>
-  <si>
-    <t>To : 26-04-2019</t>
+    <t>From : 01-10-2018</t>
+  </si>
+  <si>
+    <t>To : 30-04-2019</t>
   </si>
   <si>
     <t xml:space="preserve">Denomination : </t>
@@ -86,7 +86,7 @@
     <t>Print taken by : Satya</t>
   </si>
   <si>
-    <t>Print taken at : 26-04-2019 14:58:22</t>
+    <t>Print taken at : 30-04-2019 14:31:48</t>
   </si>
 </sst>
 </file>

</xml_diff>